<commit_message>
Started V3 of Enclosure
</commit_message>
<xml_diff>
--- a/theory/Kinematics.xlsx
+++ b/theory/Kinematics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ondine\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261D0896-7041-4FB9-A604-C4B96EE610B5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D718350-B824-4B75-85B1-EE6638B6E21D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="240" windowWidth="18908" windowHeight="7808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,29 +242,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="22">
+  <numFmts count="21">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0\ \°"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0\ &quot;mm/s&quot;"/>
     <numFmt numFmtId="168" formatCode="0.0\ &quot;°/s&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.0\ &quot;mm&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00\ &quot;1/mm&quot;"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.00000\ &quot;°/s&quot;"/>
     <numFmt numFmtId="173" formatCode="0\ &quot;mm&quot;"/>
     <numFmt numFmtId="174" formatCode="0.00\ &quot;s&quot;"/>
-    <numFmt numFmtId="175" formatCode="0\ &quot;mm/s&quot;"/>
     <numFmt numFmtId="176" formatCode="0.000\ \°"/>
     <numFmt numFmtId="177" formatCode="0.00000"/>
     <numFmt numFmtId="178" formatCode="0.0000000"/>
     <numFmt numFmtId="179" formatCode="0.000\ &quot;mm&quot;"/>
-    <numFmt numFmtId="181" formatCode="0.0%"/>
-    <numFmt numFmtId="182" formatCode="0.000000000000"/>
-    <numFmt numFmtId="183" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="184" formatCode="0.00000\ &quot;1/s&quot;"/>
-    <numFmt numFmtId="189" formatCode="0.000\ &quot;rev/s&quot;"/>
+    <numFmt numFmtId="180" formatCode="0.0%"/>
+    <numFmt numFmtId="181" formatCode="0.000000000000"/>
+    <numFmt numFmtId="182" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="183" formatCode="0.00000\ &quot;1/s&quot;"/>
+    <numFmt numFmtId="184" formatCode="0.000\ &quot;rev/s&quot;"/>
+    <numFmt numFmtId="187" formatCode="0.000\ &quot;m&quot;"/>
+    <numFmt numFmtId="190" formatCode="0.000\ &quot;m/s&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -460,7 +459,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -492,7 +490,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -512,7 +509,6 @@
     <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -531,23 +527,26 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="184" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="183" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -19292,7 +19291,7 @@
   <dimension ref="A3:Q94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19324,358 +19323,358 @@
       <c r="B11" s="2">
         <v>45</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
-      <c r="B12" s="9">
-        <v>90</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="76">
+        <v>0.09</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
-      <c r="B13" s="9">
-        <v>35</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="76">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="47">
         <v>0.01</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A17" s="20"/>
-      <c r="B17" s="41">
+      <c r="A17" s="19"/>
+      <c r="B17" s="39">
         <v>1000</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="F17" s="15"/>
+      <c r="D17" s="22"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="15"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A18" s="20"/>
-      <c r="B18" s="41">
+      <c r="A18" s="19"/>
+      <c r="B18" s="39">
         <v>1000</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A19" s="20"/>
-      <c r="B19" s="41">
+      <c r="A19" s="19"/>
+      <c r="B19" s="39">
         <v>50</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="23"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A20" s="20"/>
-      <c r="B20" s="41">
+      <c r="A20" s="19"/>
+      <c r="B20" s="39">
         <v>0</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="23"/>
+      <c r="D20" s="22"/>
     </row>
     <row r="21" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="24"/>
-      <c r="B21" s="32">
+      <c r="A21" s="23"/>
+      <c r="B21" s="31">
         <v>10</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="27"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="39"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="39"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="37"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="19"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="56">
+      <c r="B24" s="53">
         <f>B21*B14</f>
         <v>0.1</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="23"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A25" s="20"/>
-      <c r="B25" s="59">
+      <c r="A25" s="19"/>
+      <c r="B25" s="56">
         <v>48</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="24"/>
-      <c r="B26" s="60">
+      <c r="A26" s="23"/>
+      <c r="B26" s="57">
         <f>B19*B90+B20*D90</f>
         <v>8.7266418294915438E-2</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="19"/>
-      <c r="G28" s="50" t="s">
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="18"/>
+      <c r="G28" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="19"/>
-      <c r="N28" s="50" t="s">
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="18"/>
+      <c r="N28" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="O28" s="19"/>
+      <c r="O28" s="18"/>
     </row>
     <row r="29" spans="1:15" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A29" s="30"/>
-      <c r="B29" s="51">
-        <v>1</v>
-      </c>
-      <c r="C29" s="22" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="77">
+        <v>1E-3</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21">
+      <c r="D29" s="22"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20">
         <f>DEGREES(G67*B29+H67*B30+I67*RADIANS(B31))</f>
         <v>-1.1575495493448507</v>
       </c>
-      <c r="I29" s="77">
+      <c r="I29" s="74">
         <f>H29/360</f>
         <v>-3.2154154148468072E-3</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="75"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="33">
+      <c r="K29" s="22"/>
+      <c r="L29" s="72"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="78">
         <f>RADIANS(G80*H29+H80*H30+I80*H31)</f>
-        <v>1.0000000000000002</v>
+        <v>1.0000000000000002E-3</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A30" s="30"/>
-      <c r="B30" s="51">
+      <c r="A30" s="29"/>
+      <c r="B30" s="77">
         <v>0</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="22"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21">
+      <c r="G30" s="19"/>
+      <c r="H30" s="20">
         <f>DEGREES(G68*B29+H68*B30+I68*RADIANS(B31))</f>
         <v>0.57877477467242533</v>
       </c>
-      <c r="I30" s="77">
+      <c r="I30" s="74">
         <f>H30/360</f>
         <v>1.6077077074234036E-3</v>
       </c>
-      <c r="J30" s="22" t="s">
+      <c r="J30" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="23"/>
-      <c r="L30" s="75"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="33">
+      <c r="K30" s="22"/>
+      <c r="L30" s="72"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="78">
         <f>RADIANS((G81*H29+H81*H30+I81*H31))</f>
-        <v>1.2401310215141802E-16</v>
+        <v>6.0553272534872081E-20</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31">
         <v>0</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="25">
+      <c r="D31" s="26"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="24">
         <f>DEGREES(G69*B29+H69*B30+I69*RADIANS(B31))</f>
         <v>0.57877477467242533</v>
       </c>
-      <c r="I31" s="78">
+      <c r="I31" s="75">
         <f>H31/360</f>
         <v>1.6077077074234036E-3</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="27"/>
-      <c r="L31" s="75"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="34">
+      <c r="K31" s="26"/>
+      <c r="L31" s="72"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="32">
         <f>(K82*H29+L82*H30+M82*H31)/B12</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="40"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="13"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="42"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="12"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="40"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="19"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="13"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="18"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="12"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="40"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A34" s="46"/>
-      <c r="B34" s="41">
+      <c r="A34" s="44"/>
+      <c r="B34" s="39">
         <f>B17+B19</f>
         <v>1050</v>
       </c>
-      <c r="C34" s="52" t="s">
+      <c r="C34" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="13"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="42"/>
+      <c r="D34" s="22"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="12"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="40"/>
     </row>
     <row r="35" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="47"/>
-      <c r="B35" s="48">
+      <c r="A35" s="45"/>
+      <c r="B35" s="46">
         <f>B18+B20</f>
         <v>1000</v>
       </c>
-      <c r="C35" s="53" t="s">
+      <c r="C35" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="13"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="42"/>
+      <c r="D35" s="26"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="12"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="40"/>
     </row>
     <row r="36" spans="1:17" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A36" s="40"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="13"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="42"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="12"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="40"/>
     </row>
     <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="34"/>
     </row>
     <row r="39" spans="1:17" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A39" s="30"/>
-      <c r="B39" s="37">
+      <c r="A39" s="29"/>
+      <c r="B39" s="35">
         <v>0</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="7">
         <f>SIN(RADIANS(B39))</f>
         <v>0</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="7">
@@ -19684,18 +19683,18 @@
       </c>
     </row>
     <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="31"/>
-      <c r="B40" s="38">
+      <c r="A40" s="30"/>
+      <c r="B40" s="36">
         <v>0</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="7">
         <f>SIN(RADIANS(B40))</f>
         <v>0</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F40" s="7">
@@ -19711,99 +19710,99 @@
         <v>48</v>
       </c>
       <c r="B43" s="3"/>
-      <c r="F43" s="72">
+      <c r="F43" s="69">
         <v>0</v>
       </c>
-      <c r="G43" s="73">
+      <c r="G43" s="70">
         <f>-1/(B13)*COS(RADIANS(B11))</f>
-        <v>-2.0203050891044214E-2</v>
-      </c>
-      <c r="H43" s="74">
+        <v>-20.203050891044214</v>
+      </c>
+      <c r="H43" s="71">
         <f>1/(B13)*SIN(RADIANS(B11))</f>
-        <v>2.0203050891044214E-2</v>
-      </c>
-      <c r="N43" s="72">
+        <v>20.20305089104421</v>
+      </c>
+      <c r="N43" s="69">
         <f t="array" ref="N43:P45">MINVERSE(F43:H45)</f>
-        <v>6.3454531257157525E-15</v>
-      </c>
-      <c r="O43" s="62">
-        <v>28.577380332470412</v>
-      </c>
-      <c r="P43" s="63">
-        <v>-28.577380332470412</v>
+        <v>3.1727265628578762E-18</v>
+      </c>
+      <c r="O43" s="59">
+        <v>2.8577380332470412E-2</v>
+      </c>
+      <c r="P43" s="60">
+        <v>-2.8577380332470412E-2</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="E44" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="72">
+      <c r="F44" s="69">
         <f>1/(B13)*SQRT(3)/2*COS(RADIANS(B11))</f>
-        <v>1.7496355305594128E-2</v>
-      </c>
-      <c r="G44" s="73">
+        <v>17.496355305594129</v>
+      </c>
+      <c r="G44" s="70">
         <f>1/(B13)*COS(RADIANS(B11))/2</f>
-        <v>1.0101525445522107E-2</v>
-      </c>
-      <c r="H44" s="74">
+        <v>10.101525445522107</v>
+      </c>
+      <c r="H44" s="71">
         <f>1/(B13)*SIN(RADIANS(B11))</f>
-        <v>2.0203050891044214E-2</v>
+        <v>20.20305089104421</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="N44" s="61">
-        <v>-32.998316455372226</v>
-      </c>
-      <c r="O44" s="62">
-        <v>16.49915822768611</v>
-      </c>
-      <c r="P44" s="63">
-        <v>16.49915822768611</v>
+      <c r="N44" s="58">
+        <v>-3.2998316455372226E-2</v>
+      </c>
+      <c r="O44" s="59">
+        <v>1.6499158227686109E-2</v>
+      </c>
+      <c r="P44" s="60">
+        <v>1.6499158227686109E-2</v>
       </c>
       <c r="Q44" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="F45" s="72">
+      <c r="F45" s="69">
         <f>-1/(B13)*SQRT(3)/2*COS(RADIANS(B11))</f>
-        <v>-1.7496355305594128E-2</v>
-      </c>
-      <c r="G45" s="73">
+        <v>-17.496355305594129</v>
+      </c>
+      <c r="G45" s="70">
         <f>1/(B13)*COS(RADIANS(B11))/2</f>
-        <v>1.0101525445522107E-2</v>
-      </c>
-      <c r="H45" s="74">
+        <v>10.101525445522107</v>
+      </c>
+      <c r="H45" s="71">
         <f>1/(B13)*SIN(RADIANS(B11))</f>
-        <v>2.0203050891044214E-2</v>
-      </c>
-      <c r="N45" s="61">
-        <v>16.49915822768611</v>
-      </c>
-      <c r="O45" s="62">
-        <v>16.49915822768611</v>
-      </c>
-      <c r="P45" s="63">
-        <v>16.49915822768611</v>
+        <v>20.20305089104421</v>
+      </c>
+      <c r="N45" s="58">
+        <v>1.6499158227686113E-2</v>
+      </c>
+      <c r="O45" s="59">
+        <v>1.6499158227686113E-2</v>
+      </c>
+      <c r="P45" s="60">
+        <v>1.6499158227686113E-2</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="F48" s="68">
+      <c r="F48" s="65">
         <v>0</v>
       </c>
-      <c r="G48" s="69">
+      <c r="G48" s="66">
         <v>-1</v>
       </c>
-      <c r="H48" s="70">
+      <c r="H48" s="67">
         <v>0</v>
       </c>
-      <c r="N48" s="61">
+      <c r="N48" s="58">
         <f t="array" ref="N48:P50">MINVERSE(F48:H50)</f>
         <v>0</v>
       </c>
-      <c r="O48" s="62">
+      <c r="O48" s="59">
         <v>1</v>
       </c>
-      <c r="P48" s="63">
+      <c r="P48" s="60">
         <v>0</v>
       </c>
     </row>
@@ -19811,58 +19810,58 @@
       <c r="C49" t="s">
         <v>2</v>
       </c>
-      <c r="F49" s="68">
+      <c r="F49" s="65">
         <v>1</v>
       </c>
-      <c r="G49" s="69">
+      <c r="G49" s="66">
         <v>0</v>
       </c>
-      <c r="H49" s="70">
+      <c r="H49" s="67">
         <v>0</v>
       </c>
-      <c r="N49" s="61">
+      <c r="N49" s="58">
         <v>-1</v>
       </c>
-      <c r="O49" s="62">
+      <c r="O49" s="59">
         <v>0</v>
       </c>
-      <c r="P49" s="63">
+      <c r="P49" s="60">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="F50" s="68">
+      <c r="F50" s="65">
         <v>0</v>
       </c>
-      <c r="G50" s="69">
+      <c r="G50" s="66">
         <v>0</v>
       </c>
-      <c r="H50" s="70">
+      <c r="H50" s="67">
         <f>-B12</f>
-        <v>-90</v>
-      </c>
-      <c r="N50" s="61">
+        <v>-0.09</v>
+      </c>
+      <c r="N50" s="58">
         <v>0</v>
       </c>
-      <c r="O50" s="62">
+      <c r="O50" s="59">
         <v>0</v>
       </c>
-      <c r="P50" s="63">
-        <v>-1.1111111111111112E-2</v>
+      <c r="P50" s="60">
+        <v>-11.111111111111111</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>25</v>
       </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="D53" s="6"/>
@@ -19873,25 +19872,25 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-      <c r="J54" s="72">
+      <c r="J54" s="69">
         <f>F40</f>
         <v>1</v>
       </c>
-      <c r="K54" s="73">
+      <c r="K54" s="70">
         <v>0</v>
       </c>
-      <c r="L54" s="74">
+      <c r="L54" s="71">
         <f>D40</f>
         <v>0</v>
       </c>
-      <c r="N54" s="61">
+      <c r="N54" s="58">
         <f t="array" ref="N54:P56">TRANSPOSE(J54:L56)</f>
         <v>1</v>
       </c>
-      <c r="O54" s="62">
+      <c r="O54" s="59">
         <v>0</v>
       </c>
-      <c r="P54" s="63">
+      <c r="P54" s="60">
         <v>0</v>
       </c>
     </row>
@@ -19899,49 +19898,49 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
-      <c r="J55" s="72">
+      <c r="J55" s="69">
         <f>D39*D40</f>
         <v>0</v>
       </c>
-      <c r="K55" s="73">
+      <c r="K55" s="70">
         <f>F39</f>
         <v>1</v>
       </c>
-      <c r="L55" s="74">
+      <c r="L55" s="71">
         <f>-D39*F40</f>
         <v>0</v>
       </c>
-      <c r="N55" s="61">
+      <c r="N55" s="58">
         <v>0</v>
       </c>
-      <c r="O55" s="62">
+      <c r="O55" s="59">
         <v>1</v>
       </c>
-      <c r="P55" s="63">
+      <c r="P55" s="60">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="I56" s="7"/>
-      <c r="J56" s="72">
+      <c r="J56" s="69">
         <f>-F39*D40</f>
         <v>0</v>
       </c>
-      <c r="K56" s="73">
+      <c r="K56" s="70">
         <f>D39</f>
         <v>0</v>
       </c>
-      <c r="L56" s="74">
+      <c r="L56" s="71">
         <f>F39*F40</f>
         <v>1</v>
       </c>
-      <c r="N56" s="61">
+      <c r="N56" s="58">
         <v>0</v>
       </c>
-      <c r="O56" s="62">
+      <c r="O56" s="59">
         <v>0</v>
       </c>
-      <c r="P56" s="63">
+      <c r="P56" s="60">
         <v>1</v>
       </c>
     </row>
@@ -19952,7 +19951,7 @@
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
-      <c r="M57" s="14"/>
+      <c r="M57" s="13"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.45">
       <c r="D58" s="6"/>
@@ -19968,15 +19967,15 @@
       <c r="F59" s="6"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="G62" s="72">
+      <c r="G62" s="69">
         <f t="array" ref="G62:I64">MMULT(F43:H45,N54:P56)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="73">
-        <v>-2.0203050891044214E-2</v>
-      </c>
-      <c r="I62" s="74">
-        <v>2.0203050891044214E-2</v>
+      <c r="H62" s="70">
+        <v>-20.203050891044214</v>
+      </c>
+      <c r="I62" s="71">
+        <v>20.20305089104421</v>
       </c>
       <c r="K62" s="7">
         <f>F43*J54+G43*K54+H43*L54</f>
@@ -19984,61 +19983,61 @@
       </c>
       <c r="L62" s="7">
         <f>F43*J55+G43*K55+H43*L55</f>
-        <v>-2.0203050891044214E-2</v>
+        <v>-20.203050891044214</v>
       </c>
       <c r="M62" s="7">
         <f>F43*J56+G43*K56+H43*L56</f>
-        <v>2.0203050891044214E-2</v>
+        <v>20.20305089104421</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="C63" s="11"/>
+      <c r="C63" s="10"/>
       <c r="F63" t="s">
         <v>2</v>
       </c>
-      <c r="G63" s="72">
-        <v>1.7496355305594128E-2</v>
-      </c>
-      <c r="H63" s="73">
-        <v>1.0101525445522107E-2</v>
-      </c>
-      <c r="I63" s="74">
-        <v>2.0203050891044214E-2</v>
+      <c r="G63" s="69">
+        <v>17.496355305594129</v>
+      </c>
+      <c r="H63" s="70">
+        <v>10.101525445522107</v>
+      </c>
+      <c r="I63" s="71">
+        <v>20.20305089104421</v>
       </c>
       <c r="K63" s="7">
         <f>F44*J54+G44*K54+H44*L54</f>
-        <v>1.7496355305594128E-2</v>
+        <v>17.496355305594129</v>
       </c>
       <c r="L63" s="7">
         <f>F44*J55+G44*K55+H44*L55</f>
-        <v>1.0101525445522107E-2</v>
+        <v>10.101525445522107</v>
       </c>
       <c r="M63" s="7">
         <f>F44*J56+G44*K56+H43*L56</f>
-        <v>2.0203050891044214E-2</v>
+        <v>20.20305089104421</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="G64" s="72">
-        <v>-1.7496355305594128E-2</v>
-      </c>
-      <c r="H64" s="73">
-        <v>1.0101525445522107E-2</v>
-      </c>
-      <c r="I64" s="74">
-        <v>2.0203050891044214E-2</v>
+      <c r="G64" s="69">
+        <v>-17.496355305594129</v>
+      </c>
+      <c r="H64" s="70">
+        <v>10.101525445522107</v>
+      </c>
+      <c r="I64" s="71">
+        <v>20.20305089104421</v>
       </c>
       <c r="K64" s="7">
         <f>F45*J54+G45*K54+H45*L54</f>
-        <v>-1.7496355305594128E-2</v>
+        <v>-17.496355305594129</v>
       </c>
       <c r="L64" s="7">
         <f>F45*J55+G45*K55+H45*L55</f>
-        <v>1.0101525445522107E-2</v>
+        <v>10.101525445522107</v>
       </c>
       <c r="M64" s="7">
         <f>F45*J56+G45*K56+H43*L56</f>
-        <v>2.0203050891044214E-2</v>
+        <v>20.20305089104421</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.45">
@@ -20048,19 +20047,19 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" s="8"/>
-      <c r="G67" s="61">
+      <c r="G67" s="58">
         <f t="array" ref="G67:I69">MMULT(G62:I64,F48:H50)</f>
-        <v>-2.0203050891044214E-2</v>
-      </c>
-      <c r="H67" s="62">
+        <v>-20.203050891044214</v>
+      </c>
+      <c r="H67" s="59">
         <v>0</v>
       </c>
-      <c r="I67" s="63">
-        <v>-1.8182745801939793</v>
+      <c r="I67" s="60">
+        <v>-1.8182745801939788</v>
       </c>
       <c r="K67" s="7">
         <f>G43*K55+H43*L55</f>
-        <v>-2.0203050891044214E-2</v>
+        <v>-20.203050891044214</v>
       </c>
       <c r="L67" s="7">
         <f>-(H43*L54)</f>
@@ -20068,91 +20067,91 @@
       </c>
       <c r="M67" s="7">
         <f>(G43*K56+H43*L56)*H50</f>
-        <v>-1.8182745801939793</v>
+        <v>-1.8182745801939788</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="F68" s="14" t="s">
+      <c r="F68" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G68" s="61">
-        <v>1.0101525445522107E-2</v>
-      </c>
-      <c r="H68" s="62">
-        <v>-1.7496355305594128E-2</v>
-      </c>
-      <c r="I68" s="63">
-        <v>-1.8182745801939793</v>
+      <c r="G68" s="58">
+        <v>10.101525445522107</v>
+      </c>
+      <c r="H68" s="59">
+        <v>-17.496355305594129</v>
+      </c>
+      <c r="I68" s="60">
+        <v>-1.8182745801939788</v>
       </c>
       <c r="K68" s="7">
         <f>F44*J55+G44*K55+H43*L55</f>
-        <v>1.0101525445522107E-2</v>
+        <v>10.101525445522107</v>
       </c>
       <c r="L68" s="7">
         <f>-F44*J54-H43*L54</f>
-        <v>-1.7496355305594128E-2</v>
+        <v>-17.496355305594129</v>
       </c>
       <c r="M68" s="7">
         <f>(F44*J56+G44*K56+H43*L56)*H50</f>
-        <v>-1.8182745801939793</v>
+        <v>-1.8182745801939788</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G69" s="61">
-        <v>1.0101525445522107E-2</v>
-      </c>
-      <c r="H69" s="62">
-        <v>1.7496355305594128E-2</v>
-      </c>
-      <c r="I69" s="63">
-        <v>-1.8182745801939793</v>
+      <c r="G69" s="58">
+        <v>10.101525445522107</v>
+      </c>
+      <c r="H69" s="59">
+        <v>17.496355305594129</v>
+      </c>
+      <c r="I69" s="60">
+        <v>-1.8182745801939788</v>
       </c>
       <c r="K69" s="7">
         <f>-F44*J55+G44*K55+H43*L55</f>
-        <v>1.0101525445522107E-2</v>
+        <v>10.101525445522107</v>
       </c>
       <c r="L69" s="7">
         <f>F44*J54-H43*L54</f>
-        <v>1.7496355305594128E-2</v>
+        <v>17.496355305594129</v>
       </c>
       <c r="M69" s="7">
         <f>(-F44*J56+G44*K56+H43*L56)*H50</f>
-        <v>-1.8182745801939793</v>
+        <v>-1.8182745801939788</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.45">
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="71"/>
-      <c r="M71" s="16"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="68"/>
+      <c r="M71" s="15"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
-      <c r="K72" s="16"/>
-      <c r="L72" s="16"/>
-      <c r="M72" s="16"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
-      <c r="M73" s="16"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G75" s="72">
+      <c r="G75" s="69">
         <f t="array" ref="G75:I77">MMULT(N48:P50,J54:L56)</f>
         <v>0</v>
       </c>
-      <c r="H75" s="73">
+      <c r="H75" s="70">
         <v>1</v>
       </c>
-      <c r="I75" s="74">
+      <c r="I75" s="71">
         <v>0</v>
       </c>
       <c r="K75" s="7">
@@ -20169,13 +20168,13 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G76" s="72">
+      <c r="G76" s="69">
         <v>-1</v>
       </c>
-      <c r="H76" s="73">
+      <c r="H76" s="70">
         <v>0</v>
       </c>
-      <c r="I76" s="74">
+      <c r="I76" s="71">
         <v>0</v>
       </c>
       <c r="K76" s="7">
@@ -20192,14 +20191,14 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G77" s="72">
+      <c r="G77" s="69">
         <v>0</v>
       </c>
-      <c r="H77" s="73">
+      <c r="H77" s="70">
         <v>0</v>
       </c>
-      <c r="I77" s="74">
-        <v>-1.1111111111111112E-2</v>
+      <c r="I77" s="71">
+        <v>-11.111111111111111</v>
       </c>
       <c r="K77" s="7">
         <f>-J56/B12</f>
@@ -20211,7 +20210,7 @@
       </c>
       <c r="M77" s="7">
         <f>-L56/B12</f>
-        <v>-1.1111111111111112E-2</v>
+        <v>-11.111111111111111</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.45">
@@ -20223,38 +20222,38 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G80" s="61">
+      <c r="G80" s="58">
         <f t="array" ref="G80:I82">MMULT(G75:I77,N43:P45)</f>
-        <v>-32.998316455372226</v>
-      </c>
-      <c r="H80" s="62">
-        <v>16.49915822768611</v>
-      </c>
-      <c r="I80" s="63">
-        <v>16.49915822768611</v>
+        <v>-3.2998316455372226E-2</v>
+      </c>
+      <c r="H80" s="59">
+        <v>1.6499158227686109E-2</v>
+      </c>
+      <c r="I80" s="60">
+        <v>1.6499158227686109E-2</v>
       </c>
       <c r="K80" s="7">
         <f>(K55*N44+L55*N45)</f>
-        <v>-32.998316455372226</v>
+        <v>-3.2998316455372226E-2</v>
       </c>
       <c r="L80" s="7">
         <f>(J55*O43+K55*O44+L55*N45)</f>
-        <v>16.49915822768611</v>
+        <v>1.6499158227686109E-2</v>
       </c>
       <c r="M80" s="7">
         <f>(-J55*O43+K55*O44+L55*N45)</f>
-        <v>16.49915822768611</v>
+        <v>1.6499158227686109E-2</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G81" s="61">
-        <v>-6.3454531257157525E-15</v>
-      </c>
-      <c r="H81" s="62">
-        <v>-28.577380332470412</v>
-      </c>
-      <c r="I81" s="63">
-        <v>28.577380332470412</v>
+      <c r="G81" s="58">
+        <v>-3.1727265628578762E-18</v>
+      </c>
+      <c r="H81" s="59">
+        <v>-2.8577380332470412E-2</v>
+      </c>
+      <c r="I81" s="60">
+        <v>2.8577380332470412E-2</v>
       </c>
       <c r="K81" s="7">
         <f>(-L54*N45)</f>
@@ -20262,34 +20261,34 @@
       </c>
       <c r="L81" s="7">
         <f>(-J54*O43-L54*N45)</f>
-        <v>-28.577380332470412</v>
+        <v>-2.8577380332470412E-2</v>
       </c>
       <c r="M81" s="7">
         <f>(J54*O43-L54*N45)</f>
-        <v>28.577380332470412</v>
+        <v>2.8577380332470412E-2</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G82" s="61">
-        <v>-0.18332398030762345</v>
-      </c>
-      <c r="H82" s="62">
-        <v>-0.18332398030762345</v>
-      </c>
-      <c r="I82" s="63">
-        <v>-0.18332398030762345</v>
+      <c r="G82" s="58">
+        <v>-0.18332398030762348</v>
+      </c>
+      <c r="H82" s="59">
+        <v>-0.18332398030762348</v>
+      </c>
+      <c r="I82" s="60">
+        <v>-0.18332398030762348</v>
       </c>
       <c r="K82" s="7">
         <f>(-K56*N44-L56*N45)</f>
-        <v>-16.49915822768611</v>
+        <v>-1.6499158227686113E-2</v>
       </c>
       <c r="L82" s="7">
         <f>(-J56*O43-K56*O44-L56*N45)</f>
-        <v>-16.49915822768611</v>
+        <v>-1.6499158227686113E-2</v>
       </c>
       <c r="M82" s="7">
         <f>(J56*O43-K56*O44-L56*N45)</f>
-        <v>-16.49915822768611</v>
+        <v>-1.6499158227686113E-2</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.45">
@@ -20298,29 +20297,29 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D87" s="59">
+      <c r="D87" s="56">
         <f>B19*D90-B20*B90</f>
         <v>49.999923845664384</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D88" s="59">
+      <c r="D88" s="56">
         <f>B19*B90+B20*D90</f>
         <v>8.7266418294915438E-2</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B90" s="57">
+      <c r="B90" s="54">
         <f>SIN(RADIANS(B24))</f>
         <v>1.7453283658983088E-3</v>
       </c>
-      <c r="C90" s="15" t="s">
+      <c r="C90" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D90" s="58">
+      <c r="D90" s="55">
         <f>COS(RADIANS(B24))</f>
         <v>0.99999847691328769</v>
       </c>
@@ -20449,105 +20448,105 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A3" s="67">
+      <c r="A3" s="64">
         <f>SIN(RADIANS(A2))</f>
         <v>0</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="64">
         <f>SIN(RADIANS(B2))</f>
         <v>6.9756473744125302E-2</v>
       </c>
-      <c r="C3" s="67">
+      <c r="C3" s="64">
         <f t="shared" ref="C3:W3" si="1">SIN(RADIANS(C2))</f>
         <v>0.13917310096006544</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="64">
         <f t="shared" si="1"/>
         <v>0.20791169081775934</v>
       </c>
-      <c r="E3" s="67">
+      <c r="E3" s="64">
         <f t="shared" si="1"/>
         <v>0.27563735581699916</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="64">
         <f t="shared" si="1"/>
         <v>0.34202014332566871</v>
       </c>
-      <c r="G3" s="67">
+      <c r="G3" s="64">
         <f t="shared" si="1"/>
         <v>0.40673664307580021</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="64">
         <f t="shared" si="1"/>
         <v>0.46947156278589081</v>
       </c>
-      <c r="I3" s="67">
+      <c r="I3" s="64">
         <f t="shared" si="1"/>
         <v>0.5299192642332049</v>
       </c>
-      <c r="J3" s="67">
+      <c r="J3" s="64">
         <f t="shared" si="1"/>
         <v>0.58778525229247314</v>
       </c>
-      <c r="K3" s="67">
+      <c r="K3" s="64">
         <f t="shared" si="1"/>
         <v>0.64278760968653925</v>
       </c>
-      <c r="L3" s="67">
+      <c r="L3" s="64">
         <f t="shared" si="1"/>
         <v>0.69465837045899725</v>
       </c>
-      <c r="M3" s="67">
+      <c r="M3" s="64">
         <f t="shared" si="1"/>
         <v>0.74314482547739424</v>
       </c>
-      <c r="N3" s="67">
+      <c r="N3" s="64">
         <f t="shared" si="1"/>
         <v>0.78801075360672201</v>
       </c>
-      <c r="O3" s="67">
+      <c r="O3" s="64">
         <f t="shared" si="1"/>
         <v>0.82903757255504174</v>
       </c>
-      <c r="P3" s="67">
+      <c r="P3" s="64">
         <f t="shared" si="1"/>
         <v>0.8660254037844386</v>
       </c>
-      <c r="Q3" s="67">
+      <c r="Q3" s="64">
         <f t="shared" si="1"/>
         <v>0.89879404629916704</v>
       </c>
-      <c r="R3" s="67">
+      <c r="R3" s="64">
         <f t="shared" si="1"/>
         <v>0.92718385456678742</v>
       </c>
-      <c r="S3" s="67">
+      <c r="S3" s="64">
         <f t="shared" si="1"/>
         <v>0.95105651629515353</v>
       </c>
-      <c r="T3" s="67">
+      <c r="T3" s="64">
         <f t="shared" si="1"/>
         <v>0.97029572627599647</v>
       </c>
-      <c r="U3" s="67">
+      <c r="U3" s="64">
         <f t="shared" si="1"/>
         <v>0.98480775301220802</v>
       </c>
-      <c r="V3" s="67">
+      <c r="V3" s="64">
         <f t="shared" si="1"/>
         <v>0.99452189536827329</v>
       </c>
-      <c r="W3" s="67">
+      <c r="W3" s="64">
         <f t="shared" si="1"/>
         <v>0.99939082701909576</v>
       </c>
-      <c r="X3" s="67">
+      <c r="X3" s="64">
         <f>X4/(2^14)</f>
         <v>1.0006103515625</v>
       </c>
-      <c r="Y3" s="67"/>
-      <c r="Z3" s="67"/>
-      <c r="AA3" s="67"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4">
@@ -20669,7 +20668,7 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <f>H4</f>
         <v>7691</v>
       </c>
@@ -20678,7 +20677,7 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <f>I4</f>
         <v>8682</v>
       </c>
@@ -20700,7 +20699,7 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="66">
+      <c r="B12" s="63">
         <f>INT(B9+B11*((B10-B9))/(2^11))</f>
         <v>8186</v>
       </c>
@@ -20710,7 +20709,7 @@
         <f>INT(SIN(RADIANS(A7))*(2^14))</f>
         <v>8192</v>
       </c>
-      <c r="C13" s="65">
+      <c r="C13" s="62">
         <f>(B12-B13)/B13</f>
         <v>-7.32421875E-4</v>
       </c>
@@ -20822,7 +20821,7 @@
         <f>INT(B29*(2^14))</f>
         <v>11272</v>
       </c>
-      <c r="E29" s="64">
+      <c r="E29" s="61">
         <f>(D28-D29)/D29</f>
         <v>-4.6132008516678496E-3</v>
       </c>
@@ -21014,7 +21013,7 @@
         <f t="shared" ref="D2:D11" si="0">(B2-$H$6)*($G$7-$G$6)/($H$7-$H$6)+$G$6</f>
         <v>255</v>
       </c>
-      <c r="E2" s="76">
+      <c r="E2" s="73">
         <f t="shared" ref="E2:E26" si="1">(D2-A2)/A2</f>
         <v>0</v>
       </c>
@@ -21025,7 +21024,7 @@
         <f>B27</f>
         <v>124</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <f t="shared" ref="I2:I7" si="2">H2/$B$2*255</f>
         <v>17.091891891891891</v>
       </c>
@@ -21053,7 +21052,7 @@
         <f t="shared" si="0"/>
         <v>251.13259668508289</v>
       </c>
-      <c r="E3" s="76">
+      <c r="E3" s="73">
         <f t="shared" si="1"/>
         <v>2.5031006877889339E-2</v>
       </c>
@@ -21064,7 +21063,7 @@
         <f>B25</f>
         <v>684</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <f t="shared" si="2"/>
         <v>94.281081081081084</v>
       </c>
@@ -21101,7 +21100,7 @@
         <f t="shared" si="0"/>
         <v>247.26519337016575</v>
       </c>
-      <c r="E4" s="76">
+      <c r="E4" s="73">
         <f t="shared" si="1"/>
         <v>5.2192312213471266E-2</v>
       </c>
@@ -21112,7 +21111,7 @@
         <f>B22</f>
         <v>1186</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <f t="shared" si="2"/>
         <v>163.47567567567569</v>
       </c>
@@ -21144,7 +21143,7 @@
         <f t="shared" si="0"/>
         <v>243.12154696132598</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="73">
         <f t="shared" si="1"/>
         <v>8.0540208717004333E-2</v>
       </c>
@@ -21155,7 +21154,7 @@
         <f>B18</f>
         <v>1475</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <f t="shared" si="2"/>
         <v>203.31081081081081</v>
       </c>
@@ -21186,7 +21185,7 @@
         <f t="shared" si="0"/>
         <v>238.97790055248618</v>
       </c>
-      <c r="E6" s="76">
+      <c r="E6" s="73">
         <f t="shared" si="1"/>
         <v>0.11152511884877291</v>
       </c>
@@ -21197,7 +21196,7 @@
         <f>B12</f>
         <v>1669</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <f t="shared" si="2"/>
         <v>230.05135135135134</v>
       </c>
@@ -21229,7 +21228,7 @@
         <f t="shared" si="0"/>
         <v>215.49723756906076</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="73">
         <f t="shared" si="1"/>
         <v>5.1206036922247601E-2</v>
       </c>
@@ -21240,7 +21239,7 @@
         <f>B2</f>
         <v>1850</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <f t="shared" si="2"/>
         <v>255</v>
       </c>
@@ -21271,7 +21270,7 @@
         <f t="shared" si="0"/>
         <v>192.01657458563537</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="73">
         <f t="shared" si="1"/>
         <v>-1.5299617509562215E-2</v>
       </c>
@@ -21303,7 +21302,7 @@
         <f t="shared" si="0"/>
         <v>184.00552486187846</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="73">
         <f t="shared" si="1"/>
         <v>-5.375541287143481E-3</v>
       </c>
@@ -21334,7 +21333,7 @@
         <f t="shared" si="0"/>
         <v>175.99447513812154</v>
       </c>
-      <c r="E10" s="76">
+      <c r="E10" s="73">
         <f t="shared" si="1"/>
         <v>5.6827150749802517E-3</v>
       </c>
@@ -21366,7 +21365,7 @@
         <f t="shared" si="0"/>
         <v>165.49723756906079</v>
       </c>
-      <c r="E11" s="76">
+      <c r="E11" s="73">
         <f t="shared" si="1"/>
         <v>3.0135610246108256E-3</v>
       </c>
@@ -21397,7 +21396,7 @@
         <f t="shared" ref="D12:D17" si="6">(B12-$H$5)*($G$6-$G$5)/($H$6-$H$5)+$G$5</f>
         <v>155</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -21430,7 +21429,7 @@
         <f t="shared" si="6"/>
         <v>147.57731958762886</v>
       </c>
-      <c r="E13" s="76">
+      <c r="E13" s="73">
         <f t="shared" si="1"/>
         <v>1.7774617845716302E-2</v>
       </c>
@@ -21462,7 +21461,7 @@
         <f t="shared" si="6"/>
         <v>140.15463917525773</v>
       </c>
-      <c r="E14" s="76">
+      <c r="E14" s="73">
         <f t="shared" si="1"/>
         <v>3.8182512409316506E-2</v>
       </c>
@@ -21495,7 +21494,7 @@
         <f t="shared" si="6"/>
         <v>130.25773195876289</v>
       </c>
-      <c r="E15" s="76">
+      <c r="E15" s="73">
         <f t="shared" si="1"/>
         <v>4.2061855670103114E-2</v>
       </c>
@@ -21527,7 +21526,7 @@
         <f t="shared" si="6"/>
         <v>120.36082474226804</v>
       </c>
-      <c r="E16" s="76">
+      <c r="E16" s="73">
         <f t="shared" si="1"/>
         <v>4.661586732406988E-2</v>
       </c>
@@ -21560,7 +21559,7 @@
         <f t="shared" si="6"/>
         <v>107.68041237113403</v>
       </c>
-      <c r="E17" s="76">
+      <c r="E17" s="73">
         <f t="shared" si="1"/>
         <v>2.5527736867943098E-2</v>
       </c>
@@ -21592,7 +21591,7 @@
         <f>(B18-$H$4)*($G$5-$G$4)/($H$5-$H$4)+$G$4</f>
         <v>95</v>
       </c>
-      <c r="E18" s="76">
+      <c r="E18" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -21624,7 +21623,7 @@
         <f>(B19-$H$4)*($G$5-$G$4)/($H$5-$H$4)+$G$4</f>
         <v>87.802768166089976</v>
       </c>
-      <c r="E19" s="76">
+      <c r="E19" s="73">
         <f t="shared" si="1"/>
         <v>3.2973743130470308E-2</v>
       </c>
@@ -21656,7 +21655,7 @@
         <f>(B20-$H$4)*($G$5-$G$4)/($H$5-$H$4)+$G$4</f>
         <v>79.913494809688586</v>
       </c>
-      <c r="E20" s="76">
+      <c r="E20" s="73">
         <f t="shared" si="1"/>
         <v>6.5513264129181153E-2</v>
       </c>
@@ -21677,7 +21676,7 @@
         <f>(B21-$H$4)*($G$5-$G$4)/($H$5-$H$4)+$G$4</f>
         <v>69.809688581314873</v>
       </c>
-      <c r="E21" s="76">
+      <c r="E21" s="73">
         <f t="shared" si="1"/>
         <v>7.3995208943305746E-2</v>
       </c>
@@ -21698,7 +21697,7 @@
         <f>(B22-$H$4)*($G$5-$G$4)/($H$5-$H$4)+$G$4</f>
         <v>55</v>
       </c>
-      <c r="E22" s="76">
+      <c r="E22" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -21719,7 +21718,7 @@
         <f>(B23-$H$3)*($G$4-$G$3)/($H$4-$H$3)+$G$3</f>
         <v>48.127490039840637</v>
       </c>
-      <c r="E23" s="76">
+      <c r="E23" s="73">
         <f t="shared" si="1"/>
         <v>6.9499778663125275E-2</v>
       </c>
@@ -21740,7 +21739,7 @@
         <f>(B24-$H$3)*($G$4-$G$3)/($H$4-$H$3)+$G$3</f>
         <v>38.625498007968126</v>
       </c>
-      <c r="E24" s="76">
+      <c r="E24" s="73">
         <f t="shared" si="1"/>
         <v>0.10358565737051789</v>
       </c>
@@ -21760,7 +21759,7 @@
         <f>(B25-$H$3)*($G$4-$G$3)/($H$4-$H$3)+$G$3</f>
         <v>25</v>
       </c>
-      <c r="E25" s="76">
+      <c r="E25" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -21780,7 +21779,7 @@
         <f t="shared" ref="D26" si="8">(B26-$H$2)*($G$3-$G$2)/($H$3-$H$2)+$G$2</f>
         <v>14.098214285714285</v>
       </c>
-      <c r="E26" s="76">
+      <c r="E26" s="73">
         <f t="shared" si="1"/>
         <v>-6.011904761904769E-2</v>
       </c>
@@ -21800,7 +21799,7 @@
         <f t="shared" ref="D27" si="9">(B27-$H$2)*($G$3-$G$2)/($H$3-$H$2)+$G$2</f>
         <v>10</v>
       </c>
-      <c r="E27" s="76">
+      <c r="E27" s="73">
         <f>(D27-A27)/A27</f>
         <v>0</v>
       </c>

</xml_diff>